<commit_message>
Fix swapped columns in spreadsheet
</commit_message>
<xml_diff>
--- a/data/statistics/2014/schoolecaresults2010-15 (2014).xlsx
+++ b/data/statistics/2014/schoolecaresults2010-15 (2014).xlsx
@@ -238,7 +238,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -493,12 +493,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -547,6 +541,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,107 +574,89 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">

</xml_diff>